<commit_message>
update decimal format in view
</commit_message>
<xml_diff>
--- a/public/assets/TemplateKelulusan.xlsx
+++ b/public/assets/TemplateKelulusan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bahan Blog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\serverc\xampp\htdocs\sialulus\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86F975D7-AF0C-4381-B821-B9B5037586DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899B4DB0-8F3C-455F-A28B-DA53022E6139}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="1" xr2:uid="{F845E2B5-6B57-447A-9216-2DE7DB5D2826}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14258" uniqueCount="2365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14261" uniqueCount="2368">
   <si>
     <t>nopesubk</t>
   </si>
@@ -7127,6 +7127,15 @@
   </si>
   <si>
     <t>2-20-16-01-00001-0320-9</t>
+  </si>
+  <si>
+    <t>jeniskelamin</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -7189,7 +7198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7197,6 +7206,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -51512,10 +51525,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA6D9C32-2350-4095-B4B6-7808C8205B5C}">
-  <dimension ref="A1:AS3"/>
+  <dimension ref="A1:AT3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -51524,12 +51537,13 @@
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.54296875" customWidth="1"/>
-    <col min="6" max="6" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.81640625" customWidth="1"/>
-    <col min="8" max="8" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.81640625" customWidth="1"/>
+    <col min="9" max="9" width="22.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -51545,128 +51559,131 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>2365</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -51683,127 +51700,130 @@
         <v>48</v>
       </c>
       <c r="F2" t="s">
+        <v>2366</v>
+      </c>
+      <c r="G2" t="s">
         <v>49</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>50</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>51</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>52</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>53</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>54</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>53</v>
       </c>
-      <c r="M2" t="s">
-        <v>55</v>
-      </c>
       <c r="N2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" t="s">
         <v>56</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>57</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>53</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>58</v>
       </c>
-      <c r="R2" t="s">
-        <v>59</v>
-      </c>
       <c r="S2" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" t="s">
         <v>53</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>60</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>61</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>62</v>
-      </c>
-      <c r="W2" t="s">
-        <v>63</v>
       </c>
       <c r="X2" t="s">
         <v>63</v>
       </c>
       <c r="Y2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z2" t="s">
         <v>62</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>64</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>56</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>65</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>57</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>53</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>56</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>66</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>67</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>68</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>56</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>57</v>
       </c>
-      <c r="AK2" t="s">
-        <v>55</v>
-      </c>
       <c r="AL2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM2" t="s">
         <v>63</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>58</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>57</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>58</v>
       </c>
-      <c r="AP2" t="s">
-        <v>55</v>
-      </c>
       <c r="AQ2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR2" t="s">
         <v>57</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>69</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>71</v>
       </c>
@@ -51820,123 +51840,126 @@
         <v>73</v>
       </c>
       <c r="F3" t="s">
+        <v>2367</v>
+      </c>
+      <c r="G3" t="s">
         <v>74</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>75</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>76</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>52</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>58</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>57</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>77</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>62</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>58</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>68</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>62</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>58</v>
       </c>
-      <c r="R3" t="s">
-        <v>59</v>
-      </c>
       <c r="S3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T3" t="s">
         <v>53</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>78</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>79</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>65</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>77</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>80</v>
       </c>
-      <c r="Y3" t="s">
-        <v>81</v>
-      </c>
       <c r="Z3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA3" t="s">
         <v>68</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>82</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>62</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>83</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>84</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>82</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>60</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>61</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>54</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>57</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>58</v>
       </c>
-      <c r="AK3" t="s">
-        <v>55</v>
-      </c>
       <c r="AL3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM3" t="s">
         <v>57</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AN3" t="s">
         <v>58</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AO3" t="s">
         <v>62</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AP3" t="s">
         <v>68</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AQ3" t="s">
         <v>85</v>
       </c>
-      <c r="AQ3" t="s">
+      <c r="AR3" t="s">
         <v>58</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="AS3" t="s">
         <v>86</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AT3" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>